<commit_message>
Updated the sanity test case for url - cnpee cnpgeneral..
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/outputData.xlsx
+++ b/src/test/resources/TestData/outputData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\train\Automation\HS_Cucumber-main\HomeserveUSA\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\train\Automation\BAU\BAU_Regression\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A0C0C5-DE1D-489C-B20E-5467F6787374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5546AE7-61AE-47C6-BC40-6E5E2C991B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{08F75E38-EE51-476C-B487-48291877C26E}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="349">
   <si>
     <t>Credit/Debit Card</t>
   </si>
@@ -669,12 +669,427 @@
   </si>
   <si>
     <t>H861964</t>
+  </si>
+  <si>
+    <t>TC_049</t>
+  </si>
+  <si>
+    <t>04/06/2024</t>
+  </si>
+  <si>
+    <t>00:03:42</t>
+  </si>
+  <si>
+    <t>kandela</t>
+  </si>
+  <si>
+    <t>19146</t>
+  </si>
+  <si>
+    <t>Auto moujjo</t>
+  </si>
+  <si>
+    <t>Testoerdrcnomq</t>
+  </si>
+  <si>
+    <t>chandra.hstest+985@gmail.com</t>
+  </si>
+  <si>
+    <t>Sale Not Completed OR UI Latency issue</t>
+  </si>
+  <si>
+    <t>TC_013</t>
+  </si>
+  <si>
+    <t>00:02:43</t>
+  </si>
+  <si>
+    <t>slwofa</t>
+  </si>
+  <si>
+    <t>64105</t>
+  </si>
+  <si>
+    <t>Auto brdyd</t>
+  </si>
+  <si>
+    <t>Testtmzgsrr</t>
+  </si>
+  <si>
+    <t>chandra.hstest+569@gmail.com</t>
+  </si>
+  <si>
+    <t>H863058</t>
+  </si>
+  <si>
+    <t>TC_050</t>
+  </si>
+  <si>
+    <t>00:04:24</t>
+  </si>
+  <si>
+    <t>charlotte-gritty</t>
+  </si>
+  <si>
+    <t>28411</t>
+  </si>
+  <si>
+    <t>Auto qkgylp</t>
+  </si>
+  <si>
+    <t>Testwfutuewjmv</t>
+  </si>
+  <si>
+    <t>chandra.hstest+798@gmail.com</t>
+  </si>
+  <si>
+    <t>H863060</t>
+  </si>
+  <si>
+    <t>TC_052</t>
+  </si>
+  <si>
+    <t>00:01:56</t>
+  </si>
+  <si>
+    <t>kingston</t>
+  </si>
+  <si>
+    <t>k7p 3a8</t>
+  </si>
+  <si>
+    <t>Auto yaegrqwqnb</t>
+  </si>
+  <si>
+    <t>Testzzzxsp</t>
+  </si>
+  <si>
+    <t>00:03:06</t>
+  </si>
+  <si>
+    <t>Auto iwtyfmjvxzys</t>
+  </si>
+  <si>
+    <t>Testwudjkepn</t>
+  </si>
+  <si>
+    <t>chandra.hstest+049@gmail.com</t>
+  </si>
+  <si>
+    <t>H863098</t>
+  </si>
+  <si>
+    <t>TC_010</t>
+  </si>
+  <si>
+    <t>00:04:40</t>
+  </si>
+  <si>
+    <t>Auto zuscydbdwiv</t>
+  </si>
+  <si>
+    <t>Testkjjmnwaxmc</t>
+  </si>
+  <si>
+    <t>chandra.hstest+006@gmail.com</t>
+  </si>
+  <si>
+    <t>H863111</t>
+  </si>
+  <si>
+    <t>00:03:54</t>
+  </si>
+  <si>
+    <t>Auto jhcncscyggki</t>
+  </si>
+  <si>
+    <t>Testvmoxxqorn</t>
+  </si>
+  <si>
+    <t>chandra.hstest+304@gmail.com</t>
+  </si>
+  <si>
+    <t>H863114</t>
+  </si>
+  <si>
+    <t>00:03:56</t>
+  </si>
+  <si>
+    <t>Auto efrjhqtgt</t>
+  </si>
+  <si>
+    <t>Testtfcmgpm</t>
+  </si>
+  <si>
+    <t>chandra.hstest+575@gmail.com</t>
+  </si>
+  <si>
+    <t>H863117</t>
+  </si>
+  <si>
+    <t>95404</t>
+  </si>
+  <si>
+    <t>00:03:17</t>
+  </si>
+  <si>
+    <t>Auto ndiyahstj</t>
+  </si>
+  <si>
+    <t>Testmtxrsajs</t>
+  </si>
+  <si>
+    <t>chandra.hstest+663@gmail.com</t>
+  </si>
+  <si>
+    <t>H863120</t>
+  </si>
+  <si>
+    <t>00:03:28</t>
+  </si>
+  <si>
+    <t>10019</t>
+  </si>
+  <si>
+    <t>Auto tckjbbls</t>
+  </si>
+  <si>
+    <t>Testojitfnnr</t>
+  </si>
+  <si>
+    <t>chandra.hstest+510@gmail.com</t>
+  </si>
+  <si>
+    <t>H863123</t>
+  </si>
+  <si>
+    <t>92545</t>
+  </si>
+  <si>
+    <t>Auto iqdgb</t>
+  </si>
+  <si>
+    <t>Testpuuyq</t>
+  </si>
+  <si>
+    <t>chandra.hstest+444@gmail.com</t>
+  </si>
+  <si>
+    <t>H863125</t>
+  </si>
+  <si>
+    <t>00:03:24</t>
+  </si>
+  <si>
+    <t>Auto deafal</t>
+  </si>
+  <si>
+    <t>Testaiemkr</t>
+  </si>
+  <si>
+    <t>chandra.hstest+209@gmail.com</t>
+  </si>
+  <si>
+    <t>H863129</t>
+  </si>
+  <si>
+    <t>00:03:27</t>
+  </si>
+  <si>
+    <t>Auto ebcnfdh</t>
+  </si>
+  <si>
+    <t>Testbbudt</t>
+  </si>
+  <si>
+    <t>chandra.hstest+929@gmail.com</t>
+  </si>
+  <si>
+    <t>H863133</t>
+  </si>
+  <si>
+    <t>00:02:59</t>
+  </si>
+  <si>
+    <t>19401</t>
+  </si>
+  <si>
+    <t>Auto nayrmo</t>
+  </si>
+  <si>
+    <t>Testyvrizncu</t>
+  </si>
+  <si>
+    <t>chandra.hstest+642@gmail.com</t>
+  </si>
+  <si>
+    <t>H863136</t>
+  </si>
+  <si>
+    <t>00:02:58</t>
+  </si>
+  <si>
+    <t>41005</t>
+  </si>
+  <si>
+    <t>Auto vtaghtyy</t>
+  </si>
+  <si>
+    <t>Testuvpbbpmdbku</t>
+  </si>
+  <si>
+    <t>chandra.hstest+371@gmail.com</t>
+  </si>
+  <si>
+    <t>H863138</t>
+  </si>
+  <si>
+    <t>00:03:15</t>
+  </si>
+  <si>
+    <t>11422</t>
+  </si>
+  <si>
+    <t>Auto wlkdaqdhfaw</t>
+  </si>
+  <si>
+    <t>Testwlggd</t>
+  </si>
+  <si>
+    <t>chandra.hstest+978@gmail.com</t>
+  </si>
+  <si>
+    <t>H863144</t>
+  </si>
+  <si>
+    <t>05/06/2024</t>
+  </si>
+  <si>
+    <t>75036</t>
+  </si>
+  <si>
+    <t>00:03:07</t>
+  </si>
+  <si>
+    <t>Auto zcjixsekn</t>
+  </si>
+  <si>
+    <t>Testmrelobomfg</t>
+  </si>
+  <si>
+    <t>chandra.hstest+926@gmail.com</t>
+  </si>
+  <si>
+    <t>H863210</t>
+  </si>
+  <si>
+    <t>TC_004</t>
+  </si>
+  <si>
+    <t>00:06:12</t>
+  </si>
+  <si>
+    <t>Auto uaaypcifz</t>
+  </si>
+  <si>
+    <t>Testtvtmfjvp</t>
+  </si>
+  <si>
+    <t>chandra.hstest+838@gmail.com</t>
+  </si>
+  <si>
+    <t>H863213</t>
+  </si>
+  <si>
+    <t>TC_053</t>
+  </si>
+  <si>
+    <t>apco-carousel</t>
+  </si>
+  <si>
+    <t>00:03:05</t>
+  </si>
+  <si>
+    <t>20176</t>
+  </si>
+  <si>
+    <t>Auto obyfcnyu</t>
+  </si>
+  <si>
+    <t>Testvlzebpsoisn</t>
+  </si>
+  <si>
+    <t>chandra.hstest+019@gmail.com</t>
+  </si>
+  <si>
+    <t>H863218</t>
+  </si>
+  <si>
+    <t>TC_055</t>
+  </si>
+  <si>
+    <t>00:02:54</t>
+  </si>
+  <si>
+    <t>cnpee</t>
+  </si>
+  <si>
+    <t>39503</t>
+  </si>
+  <si>
+    <t>Auto htcssxuuiu</t>
+  </si>
+  <si>
+    <t>Testptfdfrz</t>
+  </si>
+  <si>
+    <t>chandra.hstest+858@gmail.com</t>
+  </si>
+  <si>
+    <t>H863259</t>
+  </si>
+  <si>
+    <t>TC_057</t>
+  </si>
+  <si>
+    <t>00:07:01</t>
+  </si>
+  <si>
+    <t>cnpgeneral</t>
+  </si>
+  <si>
+    <t>39110</t>
+  </si>
+  <si>
+    <t>Auto ycpnwdrg</t>
+  </si>
+  <si>
+    <t>Testpgeqnqjzftf</t>
+  </si>
+  <si>
+    <t>H863265</t>
+  </si>
+  <si>
+    <t>00:02:55</t>
+  </si>
+  <si>
+    <t>Auto atlzewwkfqjf</t>
+  </si>
+  <si>
+    <t>Testorptvzsk</t>
+  </si>
+  <si>
+    <t>chandra.hstest+867@gmail.com</t>
+  </si>
+  <si>
+    <t>H863267</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -718,7 +1133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -741,16 +1156,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1085,26 +1514,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6C0963-9495-4890-96A6-51A15F185A08}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M35" sqref="A19:M35"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M56" sqref="A48:M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.6640625" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.88671875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.88671875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.0"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.77734375"/>
+    <col min="8" max="9" bestFit="true" customWidth="true" width="14.5546875"/>
+    <col min="10" max="10" customWidth="true" width="28.6640625"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="8.33203125"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="6.33203125"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="33.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -2376,7 +2805,7 @@
       <c r="M34" s="1"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2413,6 +2842,844 @@
         <v>16</v>
       </c>
       <c r="M35" s="1"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M37" s="1"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M40" s="1"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M41" s="1"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M42" s="1"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M43" s="1"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M44" s="1"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M45" s="1"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M46" s="1"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M47" s="1"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M48" s="1"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M50" s="1"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M51" s="1"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M52" s="1"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M53" s="1"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M54" s="1"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M55" s="1"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M56" s="1"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>337</v>
+      </c>
+      <c r="B57" t="s">
+        <v>308</v>
+      </c>
+      <c r="C57" t="s">
+        <v>344</v>
+      </c>
+      <c r="D57" t="s">
+        <v>339</v>
+      </c>
+      <c r="E57" t="s">
+        <v>340</v>
+      </c>
+      <c r="F57"/>
+      <c r="G57" t="s">
+        <v>46</v>
+      </c>
+      <c r="H57" t="s">
+        <v>345</v>
+      </c>
+      <c r="I57" t="s">
+        <v>346</v>
+      </c>
+      <c r="J57" t="s">
+        <v>347</v>
+      </c>
+      <c r="K57" t="s">
+        <v>348</v>
+      </c>
+      <c r="L57" t="s">
+        <v>16</v>
+      </c>
+      <c r="M57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated test script for albama, techupsell, fplhometech
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/outputData.xlsx
+++ b/src/test/resources/TestData/outputData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\train\Automation\BAU\BAU_Regression\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5546AE7-61AE-47C6-BC40-6E5E2C991B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C506F3A-E03A-4706-8A6E-8D58A151788A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{08F75E38-EE51-476C-B487-48291877C26E}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="400">
   <si>
     <t>Credit/Debit Card</t>
   </si>
@@ -503,9 +503,6 @@
     <t>30/05/2024</t>
   </si>
   <si>
-    <t>00:03:45</t>
-  </si>
-  <si>
     <t>Auto txacnxzafgk</t>
   </si>
   <si>
@@ -1070,26 +1067,181 @@
     <t>H863265</t>
   </si>
   <si>
-    <t>00:02:55</t>
-  </si>
-  <si>
-    <t>Auto atlzewwkfqjf</t>
-  </si>
-  <si>
-    <t>Testorptvzsk</t>
-  </si>
-  <si>
-    <t>chandra.hstest+867@gmail.com</t>
-  </si>
-  <si>
-    <t>H863267</t>
+    <t>06/06/2024</t>
+  </si>
+  <si>
+    <t>TC_059</t>
+  </si>
+  <si>
+    <t>techupsell</t>
+  </si>
+  <si>
+    <t>18224</t>
+  </si>
+  <si>
+    <t>00:03:12</t>
+  </si>
+  <si>
+    <t>Auto hycuu</t>
+  </si>
+  <si>
+    <t>Testcpvygystuwa</t>
+  </si>
+  <si>
+    <t>chandra.hstest+348@gmail.com</t>
+  </si>
+  <si>
+    <t>H863403</t>
+  </si>
+  <si>
+    <t>TC_058</t>
+  </si>
+  <si>
+    <t>00:02:50</t>
+  </si>
+  <si>
+    <t>alabama</t>
+  </si>
+  <si>
+    <t>35004</t>
+  </si>
+  <si>
+    <t>Auto hlppslmmiktq</t>
+  </si>
+  <si>
+    <t>Testzyeknamnq</t>
+  </si>
+  <si>
+    <t>chandra.hstest+032@gmail.com</t>
+  </si>
+  <si>
+    <t>H863416</t>
+  </si>
+  <si>
+    <t>TC_060</t>
+  </si>
+  <si>
+    <t>fplhometech</t>
+  </si>
+  <si>
+    <t>32927</t>
+  </si>
+  <si>
+    <t>No Payment</t>
+  </si>
+  <si>
+    <t>00:02:49</t>
+  </si>
+  <si>
+    <t>Auto gatfses</t>
+  </si>
+  <si>
+    <t>Testplvto</t>
+  </si>
+  <si>
+    <t>chandra.hstest+480@gmail.com</t>
+  </si>
+  <si>
+    <t>H863424</t>
+  </si>
+  <si>
+    <t>K1P 5A5</t>
+  </si>
+  <si>
+    <t>00:03:14</t>
+  </si>
+  <si>
+    <t>Auto ilkau</t>
+  </si>
+  <si>
+    <t>Testgparsnqojmp</t>
+  </si>
+  <si>
+    <t>chandra.hstest+614@gmail.com</t>
+  </si>
+  <si>
+    <t>H863429</t>
+  </si>
+  <si>
+    <t>00:03:19</t>
+  </si>
+  <si>
+    <t>Auto nipnfyinjmn</t>
+  </si>
+  <si>
+    <t>Testjpsyajxa</t>
+  </si>
+  <si>
+    <t>chandra.hstest+144@gmail.com</t>
+  </si>
+  <si>
+    <t>H863431</t>
+  </si>
+  <si>
+    <t>00:05:23</t>
+  </si>
+  <si>
+    <t>Auto rzfcahadvyrq</t>
+  </si>
+  <si>
+    <t>Testncdexi</t>
+  </si>
+  <si>
+    <t>chandra.hstest+750@gmail.com</t>
+  </si>
+  <si>
+    <t>H863437</t>
+  </si>
+  <si>
+    <t>TC_054</t>
+  </si>
+  <si>
+    <t>homeserve-ca</t>
+  </si>
+  <si>
+    <t>t2e0h2</t>
+  </si>
+  <si>
+    <t>00:03:00</t>
+  </si>
+  <si>
+    <t>Auto ttwzttixcmw</t>
+  </si>
+  <si>
+    <t>Testrmwtlik</t>
+  </si>
+  <si>
+    <t>chandra.hstest+206@gmail.com</t>
+  </si>
+  <si>
+    <t>H863444</t>
+  </si>
+  <si>
+    <t>TC_056</t>
+  </si>
+  <si>
+    <t>servline-water</t>
+  </si>
+  <si>
+    <t>74884</t>
+  </si>
+  <si>
+    <t>00:03:33</t>
+  </si>
+  <si>
+    <t>Auto vpxuhzljzuv</t>
+  </si>
+  <si>
+    <t>Testdddqbapi</t>
+  </si>
+  <si>
+    <t>H863466</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1173,13 +1325,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1514,26 +1669,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6C0963-9495-4890-96A6-51A15F185A08}">
-  <dimension ref="A1:M57"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M56" sqref="A48:M56"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.88671875"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.33203125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.109375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.109375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.88671875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.0"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.77734375"/>
-    <col min="8" max="9" bestFit="true" customWidth="true" width="14.5546875"/>
-    <col min="10" max="10" customWidth="true" width="28.6640625"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="8.33203125"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="6.33203125"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="33.21875"/>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -2410,8 +2565,8 @@
       <c r="B24" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>155</v>
+      <c r="C24" s="6">
+        <v>2.6041666666666665E-3</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>3</v>
@@ -2426,16 +2581,16 @@
         <v>33</v>
       </c>
       <c r="H24" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>16</v>
@@ -2450,7 +2605,7 @@
         <v>154</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>41</v>
@@ -2465,13 +2620,13 @@
         <v>0</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -2479,19 +2634,19 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>154</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>1</v>
@@ -2500,16 +2655,16 @@
         <v>0</v>
       </c>
       <c r="H26" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>16</v>
@@ -2524,7 +2679,7 @@
         <v>154</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>51</v>
@@ -2539,13 +2694,13 @@
         <v>0</v>
       </c>
       <c r="H27" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -2559,7 +2714,7 @@
         <v>154</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>18</v>
@@ -2572,16 +2727,16 @@
         <v>46</v>
       </c>
       <c r="H28" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>16</v>
@@ -2596,7 +2751,7 @@
         <v>154</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>18</v>
@@ -2609,16 +2764,16 @@
         <v>46</v>
       </c>
       <c r="H29" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>16</v>
@@ -2633,7 +2788,7 @@
         <v>154</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>24</v>
@@ -2648,16 +2803,16 @@
         <v>0</v>
       </c>
       <c r="H30" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>16</v>
@@ -2666,19 +2821,19 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>154</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -2697,7 +2852,7 @@
         <v>154</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>27</v>
@@ -2710,13 +2865,13 @@
         <v>46</v>
       </c>
       <c r="H32" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1" t="s">
@@ -2734,7 +2889,7 @@
         <v>154</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>31</v>
@@ -2749,16 +2904,16 @@
         <v>33</v>
       </c>
       <c r="H33" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>16</v>
@@ -2788,16 +2943,16 @@
         <v>0</v>
       </c>
       <c r="H34" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>16</v>
@@ -2812,7 +2967,7 @@
         <v>154</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>38</v>
@@ -2827,16 +2982,16 @@
         <v>0</v>
       </c>
       <c r="H35" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>16</v>
@@ -2845,19 +3000,19 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>1</v>
@@ -2866,37 +3021,37 @@
         <v>0</v>
       </c>
       <c r="H36" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="K36" s="1"/>
       <c r="L36" s="1" t="s">
         <v>22</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>1</v>
@@ -2905,16 +3060,16 @@
         <v>33</v>
       </c>
       <c r="H37" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>16</v>
@@ -2923,19 +3078,19 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>1</v>
@@ -2944,16 +3099,16 @@
         <v>33</v>
       </c>
       <c r="H38" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>16</v>
@@ -2962,19 +3117,19 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>1</v>
@@ -2983,10 +3138,10 @@
         <v>0</v>
       </c>
       <c r="H39" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>143</v>
@@ -2997,19 +3152,19 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>1</v>
@@ -3018,16 +3173,16 @@
         <v>33</v>
       </c>
       <c r="H40" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>16</v>
@@ -3036,19 +3191,19 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="D41" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>1</v>
@@ -3057,16 +3212,16 @@
         <v>0</v>
       </c>
       <c r="H41" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>16</v>
@@ -3075,19 +3230,19 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>1</v>
@@ -3096,16 +3251,16 @@
         <v>33</v>
       </c>
       <c r="H42" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="I42" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>16</v>
@@ -3117,10 +3272,10 @@
         <v>49</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>51</v>
@@ -3135,16 +3290,16 @@
         <v>0</v>
       </c>
       <c r="H43" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="I43" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="K43" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>16</v>
@@ -3153,19 +3308,19 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>1</v>
@@ -3174,16 +3329,16 @@
         <v>0</v>
       </c>
       <c r="H44" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="K44" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>16</v>
@@ -3195,16 +3350,16 @@
         <v>23</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>1</v>
@@ -3213,16 +3368,16 @@
         <v>0</v>
       </c>
       <c r="H45" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="J45" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="K45" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>16</v>
@@ -3234,16 +3389,16 @@
         <v>34</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>1</v>
@@ -3252,16 +3407,16 @@
         <v>0</v>
       </c>
       <c r="H46" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="I46" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="K46" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>279</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>16</v>
@@ -3273,10 +3428,10 @@
         <v>17</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>18</v>
@@ -3289,16 +3444,16 @@
         <v>46</v>
       </c>
       <c r="H47" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="I47" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="K47" s="1" t="s">
         <v>283</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>284</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>16</v>
@@ -3310,10 +3465,10 @@
         <v>20</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>18</v>
@@ -3326,16 +3481,16 @@
         <v>46</v>
       </c>
       <c r="H48" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="J48" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="K48" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>16</v>
@@ -3347,32 +3502,32 @@
         <v>26</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
         <v>46</v>
       </c>
       <c r="H49" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="J49" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>16</v>
@@ -3384,32 +3539,32 @@
         <v>43</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
         <v>46</v>
       </c>
       <c r="H50" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="I50" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="I50" s="1" t="s">
+      <c r="J50" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>301</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>16</v>
@@ -3421,16 +3576,16 @@
         <v>30</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>1</v>
@@ -3439,16 +3594,16 @@
         <v>33</v>
       </c>
       <c r="H51" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="I51" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="J51" s="1" t="s">
+      <c r="K51" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>307</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>16</v>
@@ -3460,16 +3615,16 @@
         <v>37</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>1</v>
@@ -3478,16 +3633,16 @@
         <v>0</v>
       </c>
       <c r="H52" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="I52" s="1" t="s">
+      <c r="J52" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="J52" s="1" t="s">
+      <c r="K52" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>314</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>16</v>
@@ -3496,13 +3651,13 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>316</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>3</v>
@@ -3517,16 +3672,16 @@
         <v>0</v>
       </c>
       <c r="H53" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="I53" s="1" t="s">
+      <c r="J53" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="J53" s="1" t="s">
+      <c r="K53" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>16</v>
@@ -3535,35 +3690,35 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>324</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1" t="s">
         <v>46</v>
       </c>
       <c r="H54" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I54" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="I54" s="1" t="s">
+      <c r="J54" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="J54" s="1" t="s">
+      <c r="K54" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>328</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>16</v>
@@ -3572,35 +3727,35 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>332</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
         <v>46</v>
       </c>
       <c r="H55" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="I55" s="1" t="s">
+      <c r="J55" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="J55" s="1" t="s">
+      <c r="K55" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>336</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>16</v>
@@ -3609,77 +3764,349 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
         <v>46</v>
       </c>
       <c r="H56" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="I56" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>342</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>129</v>
       </c>
       <c r="K56" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M56" s="1"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="L56" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M56" s="1"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>337</v>
-      </c>
-      <c r="B57" t="s">
-        <v>308</v>
-      </c>
-      <c r="C57" t="s">
-        <v>344</v>
-      </c>
-      <c r="D57" t="s">
-        <v>339</v>
-      </c>
-      <c r="E57" t="s">
-        <v>340</v>
-      </c>
-      <c r="F57"/>
-      <c r="G57" t="s">
-        <v>46</v>
-      </c>
-      <c r="H57" t="s">
+      <c r="C57" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="I57" t="s">
+      <c r="E57" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="J57" t="s">
-        <v>347</v>
-      </c>
-      <c r="K57" t="s">
+      <c r="F57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="L57" t="s">
-        <v>16</v>
-      </c>
-      <c r="M57"/>
+      <c r="I57" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M57" s="1"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M58" s="1"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M59" s="1"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M60" s="1"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M61" s="1"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M62" s="1"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M63" s="1"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>393</v>
+      </c>
+      <c r="B64" t="s">
+        <v>343</v>
+      </c>
+      <c r="C64" t="s">
+        <v>396</v>
+      </c>
+      <c r="D64" t="s">
+        <v>394</v>
+      </c>
+      <c r="E64" t="s">
+        <v>395</v>
+      </c>
+      <c r="F64" t="s">
+        <v>1</v>
+      </c>
+      <c r="G64" t="s">
+        <v>0</v>
+      </c>
+      <c r="H64" t="s">
+        <v>397</v>
+      </c>
+      <c r="I64" t="s">
+        <v>398</v>
+      </c>
+      <c r="J64" t="s">
+        <v>100</v>
+      </c>
+      <c r="K64" t="s">
+        <v>399</v>
+      </c>
+      <c r="L64" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>